<commit_message>
Tested MPack - ExamAdmin
</commit_message>
<xml_diff>
--- a/ExamAdmin/StudentCodes1.xlsx
+++ b/ExamAdmin/StudentCodes1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">StudentCode</t>
   </si>
@@ -29,6 +29,12 @@
   </si>
   <si>
     <t xml:space="preserve">S5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S2</t>
   </si>
 </sst>
 </file>
@@ -43,6 +49,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -63,6 +70,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,10 +141,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -159,6 +167,16 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Student Codes Change - Exam Admin
</commit_message>
<xml_diff>
--- a/ExamAdmin/StudentCodes1.xlsx
+++ b/ExamAdmin/StudentCodes1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">StudentCode</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t xml:space="preserve">S3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S5</t>
   </si>
 </sst>
 </file>
@@ -138,7 +135,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
@@ -164,11 +161,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>